<commit_message>
making progress on first report - (pandas is probably the way to go though
</commit_message>
<xml_diff>
--- a/Comp230/sales_data.xlsx
+++ b/Comp230/sales_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" state="visible" r:id="rId2"/>
@@ -283,157 +283,157 @@
     <t xml:space="preserve">223</t>
   </si>
   <si>
+    <t xml:space="preserve">224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">226</t>
+  </si>
+  <si>
+    <t xml:space="preserve">227</t>
+  </si>
+  <si>
+    <t xml:space="preserve">228</t>
+  </si>
+  <si>
+    <t xml:space="preserve">238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">229</t>
+  </si>
+  <si>
+    <t xml:space="preserve">230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/04/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">233</t>
+  </si>
+  <si>
+    <t xml:space="preserve">234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">237</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13/04/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">241</t>
+  </si>
+  <si>
+    <t xml:space="preserve">243</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14/04/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">244</t>
+  </si>
+  <si>
+    <t xml:space="preserve">245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">246</t>
+  </si>
+  <si>
+    <t xml:space="preserve">247</t>
+  </si>
+  <si>
+    <t xml:space="preserve">248</t>
+  </si>
+  <si>
+    <t xml:space="preserve">249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15/04/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">251</t>
+  </si>
+  <si>
+    <t xml:space="preserve">252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">253</t>
+  </si>
+  <si>
+    <t xml:space="preserve">254</t>
+  </si>
+  <si>
+    <t xml:space="preserve">255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">256</t>
+  </si>
+  <si>
+    <t xml:space="preserve">257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">258</t>
+  </si>
+  <si>
+    <t xml:space="preserve">259</t>
+  </si>
+  <si>
+    <t xml:space="preserve">260</t>
+  </si>
+  <si>
+    <t xml:space="preserve">261</t>
+  </si>
+  <si>
     <t xml:space="preserve">21/04/2019</t>
   </si>
   <si>
-    <t xml:space="preserve">224</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13/04/2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">225</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14/04/2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">226</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15/04/2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">227</t>
-  </si>
-  <si>
-    <t xml:space="preserve">228</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12/04/2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">238</t>
-  </si>
-  <si>
-    <t xml:space="preserve">229</t>
-  </si>
-  <si>
-    <t xml:space="preserve">230</t>
-  </si>
-  <si>
-    <t xml:space="preserve">233</t>
-  </si>
-  <si>
-    <t xml:space="preserve">234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">235</t>
+    <t xml:space="preserve">262</t>
+  </si>
+  <si>
+    <t xml:space="preserve">263</t>
+  </si>
+  <si>
+    <t xml:space="preserve">264</t>
+  </si>
+  <si>
+    <t xml:space="preserve">265</t>
+  </si>
+  <si>
+    <t xml:space="preserve">266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">267</t>
   </si>
   <si>
     <t xml:space="preserve">23/04/2019</t>
   </si>
   <si>
-    <t xml:space="preserve">236</t>
+    <t xml:space="preserve">268</t>
   </si>
   <si>
     <t xml:space="preserve">24/04/2019</t>
   </si>
   <si>
-    <t xml:space="preserve">237</t>
+    <t xml:space="preserve">269</t>
   </si>
   <si>
     <t xml:space="preserve">25/04/2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">239</t>
-  </si>
-  <si>
-    <t xml:space="preserve">240</t>
-  </si>
-  <si>
-    <t xml:space="preserve">241</t>
-  </si>
-  <si>
-    <t xml:space="preserve">243</t>
-  </si>
-  <si>
-    <t xml:space="preserve">244</t>
-  </si>
-  <si>
-    <t xml:space="preserve">245</t>
-  </si>
-  <si>
-    <t xml:space="preserve">246</t>
-  </si>
-  <si>
-    <t xml:space="preserve">247</t>
-  </si>
-  <si>
-    <t xml:space="preserve">248</t>
-  </si>
-  <si>
-    <t xml:space="preserve">249</t>
-  </si>
-  <si>
-    <t xml:space="preserve">250</t>
-  </si>
-  <si>
-    <t xml:space="preserve">251</t>
-  </si>
-  <si>
-    <t xml:space="preserve">252</t>
-  </si>
-  <si>
-    <t xml:space="preserve">253</t>
-  </si>
-  <si>
-    <t xml:space="preserve">254</t>
-  </si>
-  <si>
-    <t xml:space="preserve">255</t>
-  </si>
-  <si>
-    <t xml:space="preserve">256</t>
-  </si>
-  <si>
-    <t xml:space="preserve">257</t>
-  </si>
-  <si>
-    <t xml:space="preserve">258</t>
-  </si>
-  <si>
-    <t xml:space="preserve">259</t>
-  </si>
-  <si>
-    <t xml:space="preserve">260</t>
-  </si>
-  <si>
-    <t xml:space="preserve">261</t>
-  </si>
-  <si>
-    <t xml:space="preserve">262</t>
-  </si>
-  <si>
-    <t xml:space="preserve">263</t>
-  </si>
-  <si>
-    <t xml:space="preserve">264</t>
-  </si>
-  <si>
-    <t xml:space="preserve">265</t>
-  </si>
-  <si>
-    <t xml:space="preserve">266</t>
-  </si>
-  <si>
-    <t xml:space="preserve">267</t>
-  </si>
-  <si>
-    <t xml:space="preserve">268</t>
-  </si>
-  <si>
-    <t xml:space="preserve">269</t>
   </si>
   <si>
     <t xml:space="preserve">.</t>
@@ -556,7 +556,7 @@
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2898,8 +2898,8 @@
   </sheetPr>
   <dimension ref="A1:C1031"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2937,7 +2937,7 @@
         <v>84</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2945,10 +2945,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2956,10 +2956,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2967,10 +2967,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2978,7 +2978,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>83</v>
@@ -2989,10 +2989,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3000,10 +3000,10 @@
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3011,10 +3011,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3022,10 +3022,10 @@
         <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3033,10 +3033,10 @@
         <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3044,10 +3044,10 @@
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3055,10 +3055,10 @@
         <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3066,10 +3066,10 @@
         <v>19</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3077,10 +3077,10 @@
         <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3088,10 +3088,10 @@
         <v>21</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3099,10 +3099,10 @@
         <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3110,10 +3110,10 @@
         <v>21</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3121,10 +3121,10 @@
         <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3132,10 +3132,10 @@
         <v>25</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3143,10 +3143,10 @@
         <v>25</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3154,10 +3154,10 @@
         <v>25</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3165,10 +3165,10 @@
         <v>25</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3176,10 +3176,10 @@
         <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3187,10 +3187,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3198,10 +3198,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3209,10 +3209,10 @@
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3220,10 +3220,10 @@
         <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3231,10 +3231,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3242,10 +3242,10 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3253,10 +3253,10 @@
         <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3264,10 +3264,10 @@
         <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3275,10 +3275,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3286,10 +3286,10 @@
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3297,10 +3297,10 @@
         <v>33</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3308,10 +3308,10 @@
         <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3319,10 +3319,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3330,10 +3330,10 @@
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3341,10 +3341,10 @@
         <v>37</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3352,10 +3352,10 @@
         <v>41</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>83</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3363,10 +3363,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3374,10 +3374,10 @@
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3385,10 +3385,10 @@
         <v>45</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>89</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3396,10 +3396,10 @@
         <v>45</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3407,10 +3407,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3418,10 +3418,10 @@
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4431,7 +4431,7 @@
   <dimension ref="A1:C1019"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4518,7 +4518,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>69</v>
@@ -4529,7 +4529,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>72</v>
@@ -4540,7 +4540,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>75</v>
@@ -4551,7 +4551,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>55</v>
@@ -4562,7 +4562,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>59</v>
@@ -4573,7 +4573,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>62</v>
@@ -4584,7 +4584,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>66</v>
@@ -4595,7 +4595,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>69</v>
@@ -4606,7 +4606,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>62</v>
@@ -4617,7 +4617,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>69</v>
@@ -4628,7 +4628,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>72</v>
@@ -4639,7 +4639,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>75</v>
@@ -4650,7 +4650,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>69</v>
@@ -4661,7 +4661,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>62</v>
@@ -4672,7 +4672,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>69</v>
@@ -4683,7 +4683,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>72</v>
@@ -4694,7 +4694,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>75</v>
@@ -4705,7 +4705,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>69</v>
@@ -4716,7 +4716,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>62</v>
@@ -4727,7 +4727,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>69</v>
@@ -4738,7 +4738,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>72</v>
@@ -4749,7 +4749,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>66</v>
@@ -4760,7 +4760,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>55</v>
@@ -4771,7 +4771,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>66</v>
@@ -4782,7 +4782,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>59</v>
@@ -4793,7 +4793,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>72</v>
@@ -4804,7 +4804,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>75</v>
@@ -4815,7 +4815,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>69</v>
@@ -4826,7 +4826,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>72</v>
@@ -4837,7 +4837,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>66</v>
@@ -4848,7 +4848,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>55</v>
@@ -4859,7 +4859,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>66</v>
@@ -4870,7 +4870,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>59</v>
@@ -4881,7 +4881,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>72</v>
@@ -4892,7 +4892,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>75</v>
@@ -4903,7 +4903,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>69</v>
@@ -4914,7 +4914,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>72</v>
@@ -4925,7 +4925,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>66</v>
@@ -4936,7 +4936,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>55</v>
@@ -4947,7 +4947,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>66</v>
@@ -4958,7 +4958,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>59</v>
@@ -4969,7 +4969,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>72</v>
@@ -4980,7 +4980,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>75</v>
@@ -4991,7 +4991,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>69</v>
@@ -5002,7 +5002,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>72</v>
@@ -5013,7 +5013,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>66</v>
@@ -5024,7 +5024,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>55</v>
@@ -5035,7 +5035,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>66</v>
@@ -5046,7 +5046,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>59</v>
@@ -5057,7 +5057,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>72</v>
@@ -5068,7 +5068,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>75</v>
@@ -5079,7 +5079,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>69</v>
@@ -5090,7 +5090,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>72</v>
@@ -5101,7 +5101,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>66</v>
@@ -5112,7 +5112,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>55</v>
@@ -5123,7 +5123,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>66</v>
@@ -5134,7 +5134,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>59</v>
@@ -5145,7 +5145,7 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>62</v>
@@ -5156,7 +5156,7 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
closer to finishing report
</commit_message>
<xml_diff>
--- a/Comp230/sales_data.xlsx
+++ b/Comp230/sales_data.xlsx
@@ -14,7 +14,7 @@
     <sheet name="Inv Line Items" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="2" name="Z_9470C7F5_6080_4CDC_8533_677DB9292658_.wvu.FilterData" vbProcedure="false">Invoices!$A$1:$Z$48</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="Z_9470C7F5_6080_4CDC_8533_677DB9292658_.wvu.FilterData" vbProcedure="false">Invoices!$B$1:$Y$48</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -265,13 +265,13 @@
     <t xml:space="preserve">20</t>
   </si>
   <si>
+    <t xml:space="preserve">Invoice_ID </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
     <t xml:space="preserve">Customer_ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invoice_ID </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date</t>
   </si>
   <si>
     <t xml:space="preserve">222</t>
@@ -1755,7 +1755,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2899,12 +2899,13 @@
   <dimension ref="A1:C1031"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2920,512 +2921,512 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>135</v>
-      </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>136</v>
       </c>
     </row>
@@ -4430,7 +4431,7 @@
   </sheetPr>
   <dimension ref="A1:C1019"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
created new spreadsheet with proper formatting of numbers as numbers, strings as strings...
</commit_message>
<xml_diff>
--- a/Comp230/sales_data.xlsx
+++ b/Comp230/sales_data.xlsx
@@ -26,15 +26,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
-  <si>
-    <t xml:space="preserve">Customer_ID </t>
-  </si>
-  <si>
-    <t xml:space="preserve">First_Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last_Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+  <si>
+    <t xml:space="preserve">Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last</t>
   </si>
   <si>
     <t xml:space="preserve">Marcela</t>
@@ -94,28 +94,22 @@
     <t xml:space="preserve">Winger</t>
   </si>
   <si>
-    <t xml:space="preserve">Invoice_ID </t>
+    <t xml:space="preserve">Invoice</t>
   </si>
   <si>
     <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Customer_ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invoice_ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product_ID</t>
+    <t xml:space="preserve">Line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product</t>
   </si>
   <si>
     <t xml:space="preserve">Units</t>
   </si>
   <si>
-    <t xml:space="preserve">Product_ID </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product_Name</t>
+    <t xml:space="preserve">Name</t>
   </si>
   <si>
     <t xml:space="preserve">Price </t>
@@ -347,7 +341,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -540,7 +534,7 @@
         <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1181,7 +1175,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1191,738 +1185,937 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="1" style="1" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="2" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>222</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>1</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="D2" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>222</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>2</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="D3" s="1" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="n">
         <v>222</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="C4" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="D4" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="n">
         <v>222</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="C5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="D5" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="n">
         <v>223</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="C6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="D6" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="n">
         <v>223</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="C7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="D7" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="n">
         <v>223</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="C8" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="D8" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="n">
         <v>223</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="C9" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="D9" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="n">
         <v>224</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="C10" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="D10" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="n">
         <v>224</v>
-      </c>
-      <c r="B11" s="1" t="n">
-        <v>1</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="D11" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="n">
         <v>225</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="C12" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="D12" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="n">
         <v>225</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="C13" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C13" s="1" t="n">
+      <c r="D13" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="n">
         <v>226</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="C14" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C14" s="1" t="n">
+      <c r="D14" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="n">
         <v>226</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="C15" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C15" s="1" t="n">
+      <c r="D15" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="n">
         <v>227</v>
-      </c>
-      <c r="B16" s="1" t="n">
-        <v>3</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="D16" s="1" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="n">
         <v>228</v>
       </c>
-      <c r="B17" s="1" t="n">
+      <c r="C17" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C17" s="1" t="n">
+      <c r="D17" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="n">
         <v>228</v>
       </c>
-      <c r="B18" s="1" t="n">
+      <c r="C18" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C18" s="1" t="n">
+      <c r="D18" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="n">
         <v>229</v>
       </c>
-      <c r="B19" s="1" t="n">
+      <c r="C19" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C19" s="1" t="n">
+      <c r="D19" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="n">
         <v>229</v>
-      </c>
-      <c r="B20" s="1" t="n">
-        <v>5</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="D20" s="1" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="n">
         <v>229</v>
       </c>
-      <c r="B21" s="1" t="n">
+      <c r="C21" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C21" s="1" t="n">
+      <c r="D21" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="n">
         <v>230</v>
       </c>
-      <c r="B22" s="1" t="n">
+      <c r="C22" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C22" s="1" t="n">
+      <c r="D22" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="n">
         <v>230</v>
       </c>
-      <c r="B23" s="1" t="n">
+      <c r="C23" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C23" s="1" t="n">
+      <c r="D23" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="n">
         <v>231</v>
       </c>
-      <c r="B24" s="1" t="n">
+      <c r="C24" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C24" s="1" t="n">
+      <c r="D24" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="n">
         <v>232</v>
       </c>
-      <c r="B25" s="1" t="n">
+      <c r="C25" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C25" s="1" t="n">
+      <c r="D25" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="n">
         <v>233</v>
       </c>
-      <c r="B26" s="1" t="n">
+      <c r="C26" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C26" s="1" t="n">
+      <c r="D26" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="n">
         <v>234</v>
       </c>
-      <c r="B27" s="1" t="n">
+      <c r="C27" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C27" s="1" t="n">
+      <c r="D27" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="n">
         <v>235</v>
       </c>
-      <c r="B28" s="1" t="n">
+      <c r="C28" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C28" s="1" t="n">
+      <c r="D28" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="n">
         <v>236</v>
       </c>
-      <c r="B29" s="1" t="n">
+      <c r="C29" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C29" s="1" t="n">
+      <c r="D29" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="n">
         <v>236</v>
-      </c>
-      <c r="B30" s="1" t="n">
-        <v>1</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="D30" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="n">
         <v>237</v>
-      </c>
-      <c r="B31" s="1" t="n">
-        <v>4</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="D31" s="1" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="n">
         <v>238</v>
       </c>
-      <c r="B32" s="1" t="n">
+      <c r="C32" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C32" s="1" t="n">
+      <c r="D32" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="n">
         <v>238</v>
       </c>
-      <c r="B33" s="1" t="n">
+      <c r="C33" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C33" s="1" t="n">
+      <c r="D33" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="n">
         <v>239</v>
       </c>
-      <c r="B34" s="1" t="n">
+      <c r="C34" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C34" s="1" t="n">
+      <c r="D34" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="n">
         <v>239</v>
       </c>
-      <c r="B35" s="1" t="n">
+      <c r="C35" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C35" s="1" t="n">
+      <c r="D35" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="n">
         <v>239</v>
       </c>
-      <c r="B36" s="1" t="n">
+      <c r="C36" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C36" s="1" t="n">
+      <c r="D36" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="n">
         <v>240</v>
       </c>
-      <c r="B37" s="1" t="n">
+      <c r="C37" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C37" s="1" t="n">
+      <c r="D37" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="n">
         <v>241</v>
-      </c>
-      <c r="B38" s="1" t="n">
-        <v>1</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="D38" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="n">
         <v>242</v>
       </c>
-      <c r="B39" s="1" t="n">
+      <c r="C39" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C39" s="1" t="n">
+      <c r="D39" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="n">
         <v>243</v>
       </c>
-      <c r="B40" s="1" t="n">
+      <c r="C40" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C40" s="1" t="n">
+      <c r="D40" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="n">
         <v>244</v>
       </c>
-      <c r="B41" s="1" t="n">
+      <c r="C41" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C41" s="1" t="n">
+      <c r="D41" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="n">
         <v>244</v>
       </c>
-      <c r="B42" s="1" t="n">
+      <c r="C42" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C42" s="1" t="n">
+      <c r="D42" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="n">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="n">
         <v>245</v>
       </c>
-      <c r="B43" s="1" t="n">
+      <c r="C43" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C43" s="1" t="n">
+      <c r="D43" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="n">
         <v>245</v>
       </c>
-      <c r="B44" s="1" t="n">
+      <c r="C44" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C44" s="1" t="n">
+      <c r="D44" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="n">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="n">
         <v>246</v>
       </c>
-      <c r="B45" s="1" t="n">
+      <c r="C45" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C45" s="1" t="n">
+      <c r="D45" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="n">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="n">
         <v>247</v>
       </c>
-      <c r="B46" s="1" t="n">
+      <c r="C46" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C46" s="1" t="n">
+      <c r="D46" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="n">
         <v>248</v>
       </c>
-      <c r="B47" s="1" t="n">
+      <c r="C47" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C47" s="1" t="n">
+      <c r="D47" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="n">
         <v>249</v>
       </c>
-      <c r="B48" s="1" t="n">
+      <c r="C48" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C48" s="1" t="n">
+      <c r="D48" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="n">
         <v>250</v>
       </c>
-      <c r="B49" s="1" t="n">
+      <c r="C49" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C49" s="1" t="n">
+      <c r="D49" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="n">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="n">
         <v>251</v>
       </c>
-      <c r="B50" s="1" t="n">
+      <c r="C50" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C50" s="1" t="n">
+      <c r="D50" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="n">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="n">
         <v>252</v>
       </c>
-      <c r="B51" s="1" t="n">
+      <c r="C51" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C51" s="1" t="n">
+      <c r="D51" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="n">
+      <c r="A52" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="n">
         <v>253</v>
       </c>
-      <c r="B52" s="1" t="n">
+      <c r="C52" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C52" s="1" t="n">
+      <c r="D52" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="n">
+      <c r="A53" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="n">
         <v>254</v>
       </c>
-      <c r="B53" s="1" t="n">
+      <c r="C53" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C53" s="1" t="n">
+      <c r="D53" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="n">
+      <c r="A54" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1" t="n">
         <v>255</v>
-      </c>
-      <c r="B54" s="1" t="n">
-        <v>1</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="D54" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="n">
+      <c r="A55" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1" t="n">
         <v>256</v>
-      </c>
-      <c r="B55" s="1" t="n">
-        <v>4</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="D55" s="1" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="n">
+      <c r="A56" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1" t="n">
         <v>257</v>
       </c>
-      <c r="B56" s="1" t="n">
+      <c r="C56" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C56" s="1" t="n">
+      <c r="D56" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="n">
+      <c r="A57" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1" t="n">
         <v>258</v>
       </c>
-      <c r="B57" s="1" t="n">
+      <c r="C57" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C57" s="1" t="n">
+      <c r="D57" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="n">
+      <c r="A58" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="n">
         <v>259</v>
       </c>
-      <c r="B58" s="1" t="n">
+      <c r="C58" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C58" s="1" t="n">
+      <c r="D58" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="n">
+      <c r="A59" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1" t="n">
         <v>260</v>
       </c>
-      <c r="B59" s="1" t="n">
+      <c r="C59" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C59" s="1" t="n">
+      <c r="D59" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="n">
+      <c r="A60" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1" t="n">
         <v>261</v>
       </c>
-      <c r="B60" s="1" t="n">
+      <c r="C60" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C60" s="1" t="n">
+      <c r="D60" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="n">
+      <c r="A61" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1" t="n">
         <v>262</v>
       </c>
-      <c r="B61" s="1" t="n">
+      <c r="C61" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C61" s="1" t="n">
+      <c r="D61" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="n">
+      <c r="A62" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1" t="n">
         <v>263</v>
-      </c>
-      <c r="B62" s="1" t="n">
-        <v>1</v>
       </c>
       <c r="C62" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="D62" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="n">
+      <c r="A63" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1" t="n">
         <v>264</v>
       </c>
-      <c r="B63" s="1" t="n">
+      <c r="C63" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C63" s="1" t="n">
+      <c r="D63" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="n">
+      <c r="A64" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1" t="n">
         <v>265</v>
       </c>
-      <c r="B64" s="1" t="n">
+      <c r="C64" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C64" s="1" t="n">
+      <c r="D64" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="n">
+      <c r="A65" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" s="1" t="n">
         <v>266</v>
       </c>
-      <c r="B65" s="1" t="n">
+      <c r="C65" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C65" s="1" t="n">
+      <c r="D65" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="n">
+      <c r="A66" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1" t="n">
         <v>267</v>
       </c>
-      <c r="B66" s="1" t="n">
+      <c r="C66" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C66" s="1" t="n">
+      <c r="D66" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C68" s="0"/>
+      <c r="D68" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1945,7 +2138,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1955,16 +2148,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1972,7 +2165,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>5</v>
@@ -1986,7 +2179,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>15</v>
@@ -2000,7 +2193,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>35</v>
@@ -2014,7 +2207,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>20</v>
@@ -2028,7 +2221,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>5</v>
@@ -2042,7 +2235,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>25</v>
@@ -2056,7 +2249,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>50</v>
@@ -2070,7 +2263,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>5</v>

</xml_diff>

<commit_message>
interspersed blank rows throughout data, wrote python script to validate data
</commit_message>
<xml_diff>
--- a/Comp230/sales_data.xlsx
+++ b/Comp230/sales_data.xlsx
@@ -11,10 +11,10 @@
     <sheet name="customers" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="invoices" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="invoice line items" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="product" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="products" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="1" name="Z_9470C7F5_6080_4CDC_8533_677DB9292658_.wvu.FilterData" vbProcedure="false">invoices!$B$1:$V$48</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="Z_9470C7F5_6080_4CDC_8533_677DB9292658_.wvu.FilterData" vbProcedure="false">invoices!$B$1:$V$55</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -335,12 +335,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -383,114 +383,123 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
-        <v>125</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
-        <v>128</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="0"/>
-      <c r="E7" s="0"/>
+      <c r="A7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D9" s="0"/>
+      <c r="E9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="n">
-        <v>133</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
+        <v>131</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
+        <v>132</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>133</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
         <v>134</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -510,10 +519,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
@@ -769,63 +778,47 @@
       <c r="E21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
-        <v>242</v>
-      </c>
-      <c r="B22" s="3" t="n">
-        <v>43568</v>
-      </c>
-      <c r="C22" s="1" t="n">
-        <v>131</v>
-      </c>
+      <c r="B22" s="3"/>
       <c r="D22" s="0"/>
       <c r="E22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
-        <v>243</v>
-      </c>
-      <c r="B23" s="3" t="n">
-        <v>43569</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>130</v>
-      </c>
+      <c r="B23" s="3"/>
       <c r="D23" s="0"/>
       <c r="E23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B24" s="3" t="n">
-        <v>43570</v>
+        <v>43568</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D24" s="0"/>
       <c r="E24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B25" s="3" t="n">
-        <v>43570</v>
+        <v>43569</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D25" s="0"/>
       <c r="E25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B26" s="3" t="n">
-        <v>43571</v>
+        <v>43570</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>134</v>
@@ -835,62 +828,62 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B27" s="3" t="n">
-        <v>43571</v>
+        <v>43570</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D27" s="0"/>
       <c r="E27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B28" s="3" t="n">
-        <v>43572</v>
+        <v>43571</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D28" s="0"/>
       <c r="E28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B29" s="3" t="n">
-        <v>43573</v>
+        <v>43571</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D29" s="0"/>
       <c r="E29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B30" s="3" t="n">
-        <v>43573</v>
+        <v>43572</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D30" s="0"/>
       <c r="E30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B31" s="3" t="n">
-        <v>43574</v>
+        <v>43573</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>132</v>
@@ -900,49 +893,41 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B32" s="3" t="n">
-        <v>43574</v>
+        <v>43573</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D32" s="0"/>
       <c r="E32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
-        <v>253</v>
-      </c>
-      <c r="B33" s="3" t="n">
-        <v>43575</v>
-      </c>
-      <c r="C33" s="1" t="n">
-        <v>125</v>
-      </c>
+      <c r="B33" s="3"/>
       <c r="D33" s="0"/>
       <c r="E33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B34" s="3" t="n">
-        <v>43576</v>
+        <v>43574</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="D34" s="0"/>
       <c r="E34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B35" s="3" t="n">
-        <v>43577</v>
+        <v>43574</v>
       </c>
       <c r="C35" s="1" t="n">
         <v>128</v>
@@ -952,165 +937,224 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B36" s="3" t="n">
-        <v>43578</v>
+        <v>43575</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D36" s="0"/>
       <c r="E36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B37" s="3" t="n">
-        <v>43579</v>
+        <v>43576</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D37" s="0"/>
       <c r="E37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B38" s="3" t="n">
-        <v>43580</v>
+        <v>43577</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D38" s="0"/>
       <c r="E38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B39" s="3" t="n">
-        <v>43580</v>
+        <v>43578</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="D39" s="0"/>
       <c r="E39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B40" s="3" t="n">
-        <v>43581</v>
+        <v>43579</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D40" s="0"/>
       <c r="E40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B41" s="3" t="n">
-        <v>43582</v>
+        <v>43580</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D41" s="0"/>
       <c r="E41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
-        <v>262</v>
-      </c>
-      <c r="B42" s="3" t="n">
-        <v>43582</v>
-      </c>
-      <c r="C42" s="1" t="n">
-        <v>123</v>
-      </c>
+      <c r="B42" s="3"/>
       <c r="D42" s="0"/>
       <c r="E42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="n">
-        <v>263</v>
-      </c>
-      <c r="B43" s="3" t="n">
-        <v>43582</v>
-      </c>
-      <c r="C43" s="1" t="n">
-        <v>133</v>
-      </c>
+      <c r="B43" s="3"/>
       <c r="D43" s="0"/>
       <c r="E43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
-        <v>264</v>
-      </c>
-      <c r="B44" s="3" t="n">
-        <v>43583</v>
-      </c>
-      <c r="C44" s="1" t="n">
-        <v>124</v>
-      </c>
+      <c r="B44" s="3"/>
       <c r="D44" s="0"/>
       <c r="E44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B45" s="3" t="n">
-        <v>43585</v>
+        <v>43580</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D45" s="0"/>
       <c r="E45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B46" s="3" t="n">
-        <v>43585</v>
+        <v>43581</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="D46" s="0"/>
       <c r="E46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B47" s="3" t="n">
-        <v>43585</v>
+        <v>43582</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="D47" s="0"/>
       <c r="E47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="0"/>
+      <c r="A48" s="1" t="n">
+        <v>262</v>
+      </c>
+      <c r="B48" s="3" t="n">
+        <v>43582</v>
+      </c>
+      <c r="C48" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="D48" s="0"/>
+      <c r="E48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="0"/>
+      <c r="A49" s="1" t="n">
+        <v>263</v>
+      </c>
+      <c r="B49" s="3" t="n">
+        <v>43582</v>
+      </c>
+      <c r="C49" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="D49" s="0"/>
+      <c r="E49" s="0"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="n">
+        <v>264</v>
+      </c>
+      <c r="B50" s="3" t="n">
+        <v>43583</v>
+      </c>
+      <c r="C50" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="D50" s="0"/>
+      <c r="E50" s="0"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="3"/>
+      <c r="D51" s="0"/>
+      <c r="E51" s="0"/>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="n">
+        <v>265</v>
+      </c>
+      <c r="B52" s="3" t="n">
+        <v>43585</v>
+      </c>
+      <c r="C52" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="D52" s="0"/>
+      <c r="E52" s="0"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="n">
+        <v>266</v>
+      </c>
+      <c r="B53" s="3" t="n">
+        <v>43585</v>
+      </c>
+      <c r="C53" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="D53" s="0"/>
+      <c r="E53" s="0"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="B54" s="3" t="n">
+        <v>43585</v>
+      </c>
+      <c r="C54" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="D54" s="0"/>
+      <c r="E54" s="0"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C55" s="0"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C56" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1128,12 +1172,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1175,7 +1219,7 @@
         <v>5</v>
       </c>
       <c r="F2" s="4" t="n">
-        <f aca="false">D2*VLOOKUP(C2, product!$A$2:$C$9, 3)</f>
+        <f aca="false">D2*VLOOKUP(C2, products!$A$2:$C$9, 3)</f>
         <v>50</v>
       </c>
     </row>
@@ -1193,7 +1237,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="n">
-        <f aca="false">D3*VLOOKUP(C3, product!$A$2:$C$9, 3)</f>
+        <f aca="false">D3*VLOOKUP(C3, products!$A$2:$C$9, 3)</f>
         <v>180</v>
       </c>
       <c r="H3" s="5" t="s">
@@ -1214,885 +1258,744 @@
         <v>3</v>
       </c>
       <c r="F4" s="4" t="n">
-        <f aca="false">D4*VLOOKUP(C4, product!$A$2:$C$9, 3)</f>
+        <f aca="false">D4*VLOOKUP(C4, products!$A$2:$C$9, 3)</f>
         <v>30</v>
       </c>
       <c r="H4" s="6" t="n">
-        <f aca="false">SUM(F2:F72)</f>
+        <f aca="false">SUM(F2:F81)</f>
         <v>15020</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>222</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="F5" s="4" t="n">
-        <f aca="false">D5*VLOOKUP(C5, product!$A$2:$C$9, 3)</f>
-        <v>240</v>
-      </c>
-      <c r="H5" s="0"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F6" s="4" t="n">
-        <f aca="false">D6*VLOOKUP(C6, product!$A$2:$C$9, 3)</f>
-        <v>50</v>
-      </c>
+        <f aca="false">D6*VLOOKUP(C6, products!$A$2:$C$9, 3)</f>
+        <v>240</v>
+      </c>
+      <c r="H6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>223</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F7" s="4" t="n">
-        <f aca="false">D7*VLOOKUP(C7, product!$A$2:$C$9, 3)</f>
-        <v>560</v>
+        <f aca="false">D7*VLOOKUP(C7, products!$A$2:$C$9, 3)</f>
+        <v>50</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>223</v>
       </c>
       <c r="C8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D8" s="1" t="n">
-        <v>2</v>
-      </c>
       <c r="F8" s="4" t="n">
-        <f aca="false">D8*VLOOKUP(C8, product!$A$2:$C$9, 3)</f>
-        <v>20</v>
+        <f aca="false">D8*VLOOKUP(C8, products!$A$2:$C$9, 3)</f>
+        <v>560</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>223</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" s="4" t="n">
-        <f aca="false">D9*VLOOKUP(C9, product!$A$2:$C$9, 3)</f>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>224</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="F10" s="4" t="n">
-        <f aca="false">D10*VLOOKUP(C10, product!$A$2:$C$9, 3)</f>
-        <v>700</v>
+        <f aca="false">D9*VLOOKUP(C9, products!$A$2:$C$9, 3)</f>
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F11" s="4" t="n">
-        <f aca="false">D11*VLOOKUP(C11, product!$A$2:$C$9, 3)</f>
-        <v>50</v>
+        <f aca="false">D11*VLOOKUP(C11, products!$A$2:$C$9, 3)</f>
+        <v>150</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F12" s="4" t="n">
-        <f aca="false">D12*VLOOKUP(C12, product!$A$2:$C$9, 3)</f>
-        <v>120</v>
+        <f aca="false">D12*VLOOKUP(C12, products!$A$2:$C$9, 3)</f>
+        <v>700</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F13" s="4" t="n">
-        <f aca="false">D13*VLOOKUP(C13, product!$A$2:$C$9, 3)</f>
-        <v>210</v>
+        <f aca="false">D13*VLOOKUP(C13, products!$A$2:$C$9, 3)</f>
+        <v>50</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D14" s="1" t="n">
-        <v>5</v>
-      </c>
       <c r="F14" s="4" t="n">
-        <f aca="false">D14*VLOOKUP(C14, product!$A$2:$C$9, 3)</f>
-        <v>200</v>
+        <f aca="false">D14*VLOOKUP(C14, products!$A$2:$C$9, 3)</f>
+        <v>120</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F15" s="4" t="n">
-        <f aca="false">D15*VLOOKUP(C15, product!$A$2:$C$9, 3)</f>
-        <v>60</v>
+        <f aca="false">D15*VLOOKUP(C15, products!$A$2:$C$9, 3)</f>
+        <v>210</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F16" s="4" t="n">
-        <f aca="false">D16*VLOOKUP(C16, product!$A$2:$C$9, 3)</f>
-        <v>210</v>
+        <f aca="false">D16*VLOOKUP(C16, products!$A$2:$C$9, 3)</f>
+        <v>200</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>6</v>
       </c>
       <c r="F17" s="4" t="n">
-        <f aca="false">D17*VLOOKUP(C17, product!$A$2:$C$9, 3)</f>
+        <f aca="false">D17*VLOOKUP(C17, products!$A$2:$C$9, 3)</f>
         <v>60</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F18" s="4" t="n">
-        <f aca="false">D18*VLOOKUP(C18, product!$A$2:$C$9, 3)</f>
-        <v>250</v>
+        <f aca="false">D18*VLOOKUP(C18, products!$A$2:$C$9, 3)</f>
+        <v>210</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F19" s="4" t="n">
-        <f aca="false">D19*VLOOKUP(C19, product!$A$2:$C$9, 3)</f>
-        <v>400</v>
+        <f aca="false">D19*VLOOKUP(C19, products!$A$2:$C$9, 3)</f>
+        <v>60</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F20" s="4" t="n">
-        <f aca="false">D20*VLOOKUP(C20, product!$A$2:$C$9, 3)</f>
-        <v>90</v>
+        <f aca="false">D20*VLOOKUP(C20, products!$A$2:$C$9, 3)</f>
+        <v>250</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>229</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F21" s="4" t="n">
-        <f aca="false">D21*VLOOKUP(C21, product!$A$2:$C$9, 3)</f>
-        <v>420</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="n">
-        <v>230</v>
-      </c>
-      <c r="C22" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D22" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="F22" s="4" t="n">
-        <f aca="false">D22*VLOOKUP(C22, product!$A$2:$C$9, 3)</f>
-        <v>90</v>
+        <f aca="false">D21*VLOOKUP(C21, products!$A$2:$C$9, 3)</f>
+        <v>400</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F23" s="4" t="n">
-        <f aca="false">D23*VLOOKUP(C23, product!$A$2:$C$9, 3)</f>
-        <v>100</v>
+        <f aca="false">D23*VLOOKUP(C23, products!$A$2:$C$9, 3)</f>
+        <v>90</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F24" s="4" t="n">
-        <f aca="false">D24*VLOOKUP(C24, product!$A$2:$C$9, 3)</f>
-        <v>900</v>
+        <f aca="false">D24*VLOOKUP(C24, products!$A$2:$C$9, 3)</f>
+        <v>420</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B25" s="1" t="n">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>5</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F25" s="4" t="n">
-        <f aca="false">D25*VLOOKUP(C25, product!$A$2:$C$9, 3)</f>
-        <v>60</v>
+        <f aca="false">D25*VLOOKUP(C25, products!$A$2:$C$9, 3)</f>
+        <v>90</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B26" s="1" t="n">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" s="4" t="n">
-        <f aca="false">D26*VLOOKUP(C26, product!$A$2:$C$9, 3)</f>
-        <v>210</v>
+        <f aca="false">D26*VLOOKUP(C26, products!$A$2:$C$9, 3)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D27" s="1" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F27" s="4" t="n">
-        <f aca="false">D27*VLOOKUP(C27, product!$A$2:$C$9, 3)</f>
-        <v>60</v>
+        <f aca="false">D27*VLOOKUP(C27, products!$A$2:$C$9, 3)</f>
+        <v>900</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" s="4" t="n">
-        <f aca="false">D28*VLOOKUP(C28, product!$A$2:$C$9, 3)</f>
-        <v>350</v>
+        <f aca="false">D28*VLOOKUP(C28, products!$A$2:$C$9, 3)</f>
+        <v>60</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" s="4" t="n">
-        <f aca="false">D29*VLOOKUP(C29, product!$A$2:$C$9, 3)</f>
-        <v>160</v>
+        <f aca="false">D29*VLOOKUP(C29, products!$A$2:$C$9, 3)</f>
+        <v>210</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B30" s="1" t="n">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F30" s="4" t="n">
-        <f aca="false">D30*VLOOKUP(C30, product!$A$2:$C$9, 3)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B31" s="1" t="n">
-        <v>237</v>
-      </c>
-      <c r="C31" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D31" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="F31" s="4" t="n">
-        <f aca="false">D31*VLOOKUP(C31, product!$A$2:$C$9, 3)</f>
-        <v>320</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1" t="n">
-        <v>238</v>
-      </c>
-      <c r="C32" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D32" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="F32" s="4" t="n">
-        <f aca="false">D32*VLOOKUP(C32, product!$A$2:$C$9, 3)</f>
-        <v>270</v>
+        <f aca="false">D30*VLOOKUP(C30, products!$A$2:$C$9, 3)</f>
+        <v>60</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B33" s="1" t="n">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F33" s="4" t="n">
-        <f aca="false">D33*VLOOKUP(C33, product!$A$2:$C$9, 3)</f>
-        <v>60</v>
+        <f aca="false">D33*VLOOKUP(C33, products!$A$2:$C$9, 3)</f>
+        <v>350</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B34" s="1" t="n">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F34" s="4" t="n">
-        <f aca="false">D34*VLOOKUP(C34, product!$A$2:$C$9, 3)</f>
-        <v>100</v>
+        <f aca="false">D34*VLOOKUP(C34, products!$A$2:$C$9, 3)</f>
+        <v>160</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B35" s="1" t="n">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D35" s="1" t="n">
         <v>5</v>
       </c>
       <c r="F35" s="4" t="n">
-        <f aca="false">D35*VLOOKUP(C35, product!$A$2:$C$9, 3)</f>
+        <f aca="false">D35*VLOOKUP(C35, products!$A$2:$C$9, 3)</f>
         <v>50</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B36" s="1" t="n">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F36" s="4" t="n">
-        <f aca="false">D36*VLOOKUP(C36, product!$A$2:$C$9, 3)</f>
-        <v>450</v>
+        <f aca="false">D36*VLOOKUP(C36, products!$A$2:$C$9, 3)</f>
+        <v>320</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B37" s="1" t="n">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F37" s="4" t="n">
-        <f aca="false">D37*VLOOKUP(C37, product!$A$2:$C$9, 3)</f>
-        <v>240</v>
+        <f aca="false">D37*VLOOKUP(C37, products!$A$2:$C$9, 3)</f>
+        <v>270</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B38" s="1" t="n">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F38" s="4" t="n">
-        <f aca="false">D38*VLOOKUP(C38, product!$A$2:$C$9, 3)</f>
-        <v>20</v>
+        <f aca="false">D38*VLOOKUP(C38, products!$A$2:$C$9, 3)</f>
+        <v>60</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B39" s="1" t="n">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F39" s="4" t="n">
-        <f aca="false">D39*VLOOKUP(C39, product!$A$2:$C$9, 3)</f>
-        <v>200</v>
+        <f aca="false">D39*VLOOKUP(C39, products!$A$2:$C$9, 3)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B40" s="1" t="n">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D40" s="1" t="n">
         <v>5</v>
       </c>
       <c r="F40" s="4" t="n">
-        <f aca="false">D40*VLOOKUP(C40, product!$A$2:$C$9, 3)</f>
-        <v>150</v>
+        <f aca="false">D40*VLOOKUP(C40, products!$A$2:$C$9, 3)</f>
+        <v>50</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B41" s="1" t="n">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C41" s="1" t="n">
         <v>6</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F41" s="4" t="n">
-        <f aca="false">D41*VLOOKUP(C41, product!$A$2:$C$9, 3)</f>
-        <v>300</v>
+        <f aca="false">D41*VLOOKUP(C41, products!$A$2:$C$9, 3)</f>
+        <v>450</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B42" s="1" t="n">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F42" s="4" t="n">
-        <f aca="false">D42*VLOOKUP(C42, product!$A$2:$C$9, 3)</f>
-        <v>500</v>
+        <f aca="false">D42*VLOOKUP(C42, products!$A$2:$C$9, 3)</f>
+        <v>240</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B43" s="1" t="n">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F43" s="4" t="n">
-        <f aca="false">D43*VLOOKUP(C43, product!$A$2:$C$9, 3)</f>
-        <v>80</v>
+        <f aca="false">D43*VLOOKUP(C43, products!$A$2:$C$9, 3)</f>
+        <v>20</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B44" s="1" t="n">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D44" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F44" s="4" t="n">
-        <f aca="false">D44*VLOOKUP(C44, product!$A$2:$C$9, 3)</f>
-        <v>450</v>
+        <f aca="false">D44*VLOOKUP(C44, products!$A$2:$C$9, 3)</f>
+        <v>200</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B45" s="1" t="n">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D45" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F45" s="4" t="n">
-        <f aca="false">D45*VLOOKUP(C45, product!$A$2:$C$9, 3)</f>
-        <v>240</v>
+        <f aca="false">D45*VLOOKUP(C45, products!$A$2:$C$9, 3)</f>
+        <v>150</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B46" s="1" t="n">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D46" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F46" s="4" t="n">
-        <f aca="false">D46*VLOOKUP(C46, product!$A$2:$C$9, 3)</f>
-        <v>70</v>
+        <f aca="false">D46*VLOOKUP(C46, products!$A$2:$C$9, 3)</f>
+        <v>300</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B47" s="1" t="n">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D47" s="1" t="n">
         <v>5</v>
       </c>
       <c r="F47" s="4" t="n">
-        <f aca="false">D47*VLOOKUP(C47, product!$A$2:$C$9, 3)</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="B48" s="1" t="n">
-        <v>249</v>
-      </c>
-      <c r="C48" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D48" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="F48" s="4" t="n">
-        <f aca="false">D48*VLOOKUP(C48, product!$A$2:$C$9, 3)</f>
-        <v>270</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B49" s="1" t="n">
-        <v>250</v>
-      </c>
-      <c r="C49" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="D49" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="F49" s="4" t="n">
-        <f aca="false">D49*VLOOKUP(C49, product!$A$2:$C$9, 3)</f>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B50" s="1" t="n">
-        <v>251</v>
-      </c>
-      <c r="C50" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="D50" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="F50" s="4" t="n">
-        <f aca="false">D50*VLOOKUP(C50, product!$A$2:$C$9, 3)</f>
+        <f aca="false">D47*VLOOKUP(C47, products!$A$2:$C$9, 3)</f>
         <v>500</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B51" s="1" t="n">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D51" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F51" s="4" t="n">
-        <f aca="false">D51*VLOOKUP(C51, product!$A$2:$C$9, 3)</f>
-        <v>60</v>
+        <f aca="false">D51*VLOOKUP(C51, products!$A$2:$C$9, 3)</f>
+        <v>80</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B52" s="1" t="n">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F52" s="4" t="n">
-        <f aca="false">D52*VLOOKUP(C52, product!$A$2:$C$9, 3)</f>
-        <v>70</v>
+        <f aca="false">D52*VLOOKUP(C52, products!$A$2:$C$9, 3)</f>
+        <v>450</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B53" s="1" t="n">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>4</v>
@@ -2101,52 +2004,52 @@
         <v>6</v>
       </c>
       <c r="F53" s="4" t="n">
-        <f aca="false">D53*VLOOKUP(C53, product!$A$2:$C$9, 3)</f>
+        <f aca="false">D53*VLOOKUP(C53, products!$A$2:$C$9, 3)</f>
         <v>240</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B54" s="1" t="n">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F54" s="4" t="n">
-        <f aca="false">D54*VLOOKUP(C54, product!$A$2:$C$9, 3)</f>
-        <v>50</v>
+        <f aca="false">D54*VLOOKUP(C54, products!$A$2:$C$9, 3)</f>
+        <v>70</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B55" s="1" t="n">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D55" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F55" s="4" t="n">
-        <f aca="false">D55*VLOOKUP(C55, product!$A$2:$C$9, 3)</f>
-        <v>320</v>
+        <f aca="false">D55*VLOOKUP(C55, products!$A$2:$C$9, 3)</f>
+        <v>200</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B56" s="1" t="n">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C56" s="1" t="n">
         <v>2</v>
@@ -2155,16 +2058,16 @@
         <v>9</v>
       </c>
       <c r="F56" s="4" t="n">
-        <f aca="false">D56*VLOOKUP(C56, product!$A$2:$C$9, 3)</f>
+        <f aca="false">D56*VLOOKUP(C56, products!$A$2:$C$9, 3)</f>
         <v>270</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B57" s="1" t="n">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>6</v>
@@ -2173,88 +2076,88 @@
         <v>6</v>
       </c>
       <c r="F57" s="4" t="n">
-        <f aca="false">D57*VLOOKUP(C57, product!$A$2:$C$9, 3)</f>
+        <f aca="false">D57*VLOOKUP(C57, products!$A$2:$C$9, 3)</f>
         <v>300</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B58" s="1" t="n">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>7</v>
       </c>
       <c r="D58" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F58" s="4" t="n">
-        <f aca="false">D58*VLOOKUP(C58, product!$A$2:$C$9, 3)</f>
-        <v>700</v>
+        <f aca="false">D58*VLOOKUP(C58, products!$A$2:$C$9, 3)</f>
+        <v>500</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B59" s="1" t="n">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C59" s="1" t="n">
         <v>5</v>
       </c>
       <c r="D59" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F59" s="4" t="n">
-        <f aca="false">D59*VLOOKUP(C59, product!$A$2:$C$9, 3)</f>
-        <v>50</v>
+        <f aca="false">D59*VLOOKUP(C59, products!$A$2:$C$9, 3)</f>
+        <v>60</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B60" s="1" t="n">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D60" s="1" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F60" s="4" t="n">
-        <f aca="false">D60*VLOOKUP(C60, product!$A$2:$C$9, 3)</f>
-        <v>450</v>
+        <f aca="false">D60*VLOOKUP(C60, products!$A$2:$C$9, 3)</f>
+        <v>70</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B61" s="1" t="n">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D61" s="1" t="n">
         <v>6</v>
       </c>
       <c r="F61" s="4" t="n">
-        <f aca="false">D61*VLOOKUP(C61, product!$A$2:$C$9, 3)</f>
-        <v>60</v>
+        <f aca="false">D61*VLOOKUP(C61, products!$A$2:$C$9, 3)</f>
+        <v>240</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B62" s="1" t="n">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C62" s="1" t="n">
         <v>1</v>
@@ -2263,170 +2166,332 @@
         <v>5</v>
       </c>
       <c r="F62" s="4" t="n">
-        <f aca="false">D62*VLOOKUP(C62, product!$A$2:$C$9, 3)</f>
+        <f aca="false">D62*VLOOKUP(C62, products!$A$2:$C$9, 3)</f>
         <v>50</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B63" s="1" t="n">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C63" s="1" t="n">
         <v>4</v>
       </c>
       <c r="D63" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F63" s="4" t="n">
-        <f aca="false">D63*VLOOKUP(C63, product!$A$2:$C$9, 3)</f>
-        <v>240</v>
+        <f aca="false">D63*VLOOKUP(C63, products!$A$2:$C$9, 3)</f>
+        <v>320</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B64" s="1" t="n">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="C64" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F64" s="4" t="n">
-        <f aca="false">D64*VLOOKUP(C64, product!$A$2:$C$9, 3)</f>
-        <v>150</v>
+        <f aca="false">D64*VLOOKUP(C64, products!$A$2:$C$9, 3)</f>
+        <v>270</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B65" s="1" t="n">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D65" s="1" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F65" s="4" t="n">
-        <f aca="false">D65*VLOOKUP(C65, product!$A$2:$C$9, 3)</f>
-        <v>630</v>
+        <f aca="false">D65*VLOOKUP(C65, products!$A$2:$C$9, 3)</f>
+        <v>300</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B66" s="1" t="n">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F66" s="4" t="n">
-        <f aca="false">D66*VLOOKUP(C66, product!$A$2:$C$9, 3)</f>
-        <v>80</v>
+        <f aca="false">D66*VLOOKUP(C66, products!$A$2:$C$9, 3)</f>
+        <v>700</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="n">
+        <v>58</v>
+      </c>
       <c r="B67" s="1" t="n">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C67" s="1" t="n">
         <v>5</v>
       </c>
       <c r="D67" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F67" s="4" t="n">
-        <f aca="false">D67*VLOOKUP(C67, product!$A$2:$C$9, 3)</f>
-        <v>10</v>
+        <f aca="false">D67*VLOOKUP(C67, products!$A$2:$C$9, 3)</f>
+        <v>50</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="n">
+        <v>59</v>
+      </c>
       <c r="B68" s="1" t="n">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D68" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E68" s="0"/>
+        <v>9</v>
+      </c>
       <c r="F68" s="4" t="n">
-        <f aca="false">D68*VLOOKUP(C68, product!$A$2:$C$9, 3)</f>
-        <v>200</v>
+        <f aca="false">D68*VLOOKUP(C68, products!$A$2:$C$9, 3)</f>
+        <v>450</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="n">
+        <v>60</v>
+      </c>
       <c r="B69" s="1" t="n">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D69" s="1" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F69" s="4" t="n">
-        <f aca="false">D69*VLOOKUP(C69, product!$A$2:$C$9, 3)</f>
+        <f aca="false">D69*VLOOKUP(C69, products!$A$2:$C$9, 3)</f>
         <v>60</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="n">
+        <v>61</v>
+      </c>
       <c r="B70" s="1" t="n">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C70" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D70" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F70" s="4" t="n">
-        <f aca="false">D70*VLOOKUP(C70, product!$A$2:$C$9, 3)</f>
+        <f aca="false">D70*VLOOKUP(C70, products!$A$2:$C$9, 3)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B71" s="1" t="n">
+        <v>264</v>
+      </c>
+      <c r="C71" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D71" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="F71" s="4" t="n">
+        <f aca="false">D71*VLOOKUP(C71, products!$A$2:$C$9, 3)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B72" s="1" t="n">
+        <v>265</v>
+      </c>
+      <c r="C72" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D72" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F72" s="4" t="n">
+        <f aca="false">D72*VLOOKUP(C72, products!$A$2:$C$9, 3)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B73" s="1" t="n">
+        <v>266</v>
+      </c>
+      <c r="C73" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D73" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="F73" s="4" t="n">
+        <f aca="false">D73*VLOOKUP(C73, products!$A$2:$C$9, 3)</f>
+        <v>630</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B75" s="1" t="n">
+        <v>266</v>
+      </c>
+      <c r="C75" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D75" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F75" s="4" t="n">
+        <f aca="false">D75*VLOOKUP(C75, products!$A$2:$C$9, 3)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B76" s="1" t="n">
+        <v>266</v>
+      </c>
+      <c r="C76" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D76" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F76" s="4" t="n">
+        <f aca="false">D76*VLOOKUP(C76, products!$A$2:$C$9, 3)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B77" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="C77" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="D77" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E77" s="0"/>
+      <c r="F77" s="4" t="n">
+        <f aca="false">D77*VLOOKUP(C77, products!$A$2:$C$9, 3)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B78" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="C78" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D78" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F78" s="4" t="n">
+        <f aca="false">D78*VLOOKUP(C78, products!$A$2:$C$9, 3)</f>
         <v>60</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="1" t="n">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B79" s="1" t="n">
         <v>267</v>
       </c>
-      <c r="C71" s="1" t="n">
+      <c r="C79" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D79" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="F79" s="4" t="n">
+        <f aca="false">D79*VLOOKUP(C79, products!$A$2:$C$9, 3)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B80" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="C80" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D71" s="1" t="n">
+      <c r="D80" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F71" s="4" t="n">
-        <f aca="false">D71*VLOOKUP(C71, product!$A$2:$C$9, 3)</f>
+      <c r="F80" s="4" t="n">
+        <f aca="false">D80*VLOOKUP(C80, products!$A$2:$C$9, 3)</f>
         <v>140</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="1" t="n">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B81" s="1" t="n">
         <v>267</v>
       </c>
-      <c r="C72" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D72" s="1" t="n">
+      <c r="C81" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D81" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F72" s="4" t="n">
-        <f aca="false">D72*VLOOKUP(C72, product!$A$2:$C$9, 3)</f>
+      <c r="F81" s="4" t="n">
+        <f aca="false">D81*VLOOKUP(C81, products!$A$2:$C$9, 3)</f>
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first pass at script to merge two sales data spreadhseets, developed script to generate invoice given invoice id
</commit_message>
<xml_diff>
--- a/Comp230/sales_data.xlsx
+++ b/Comp230/sales_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="1" state="visible" r:id="rId2"/>
@@ -540,7 +540,7 @@
   </sheetPr>
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -1585,9 +1585,9 @@
   <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="F73" activeCellId="0" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2923,10 +2923,10 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
generated another month's worth of sales data for merging
</commit_message>
<xml_diff>
--- a/Comp230/sales_data.xlsx
+++ b/Comp230/sales_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="1" state="visible" r:id="rId2"/>
@@ -747,7 +747,7 @@
   </sheetPr>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -934,7 +934,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1585,9 +1585,9 @@
   <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F73" activeCellId="0" sqref="F73"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2923,10 +2923,10 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>